<commit_message>
About page documentation updates
</commit_message>
<xml_diff>
--- a/InputData/elec/BSfGBP/BAU Subsidy for Grid Battery Production.xlsx
+++ b/InputData/elec/BSfGBP/BAU Subsidy for Grid Battery Production.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\elec\BSfGBP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BSfGBP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFB4CD0-5886-4E68-825F-44BFDFD05F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE830CDA-2171-4933-BA48-7F50760EB19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59580" yWindow="1425" windowWidth="21600" windowHeight="15210" activeTab="2" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Sources:</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>In the US, the Inflation Reduction Act includes a credit of $35/kWh for battery cells and $10/kWh for assembly for grid</t>
+  </si>
+  <si>
+    <t>Policy Setting (2023 USD)</t>
+  </si>
+  <si>
+    <t>FoPITY</t>
+  </si>
+  <si>
+    <t>("Schedule 3",(2021,0),(2024,0),</t>
+  </si>
+  <si>
+    <t>(2033,0),(2050,0)),</t>
   </si>
 </sst>
 </file>
@@ -453,17 +465,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="101.26953125" customWidth="1"/>
+    <col min="2" max="2" width="101.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,37 +483,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.75350342301658668</v>
       </c>
@@ -509,7 +521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.73</v>
       </c>
@@ -517,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0.03</v>
       </c>
@@ -538,9 +550,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2023</v>
       </c>
@@ -572,7 +584,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -614,15 +626,18 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -717,7 +732,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -820,6 +835,126 @@
       </c>
       <c r="AE2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <f>F2/About!$A$12/1000</f>
+        <v>42.28846084392449</v>
+      </c>
+      <c r="G4">
+        <f>G2/About!$A$12/1000</f>
+        <v>41.019807018606755</v>
+      </c>
+      <c r="H4">
+        <f>H2/About!$A$12/1000</f>
+        <v>39.789212808048553</v>
+      </c>
+      <c r="I4">
+        <f>I2/About!$A$12/1000</f>
+        <v>38.595536423807097</v>
+      </c>
+      <c r="J4">
+        <f>J2/About!$A$12/1000</f>
+        <v>37.437670331092889</v>
+      </c>
+      <c r="K4">
+        <f>K2/About!$A$12/1000</f>
+        <v>27.235905165870069</v>
+      </c>
+      <c r="L4">
+        <f>L2/About!$A$12/1000</f>
+        <v>17.612552007262646</v>
+      </c>
+      <c r="M4">
+        <f>M2/About!$A$12/1000</f>
+        <v>8.5420877235223838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="E5:M5" si="0">F4/MAX($D$4:$M$4)</f>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.94090000000000007</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.91267300000000007</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.88529281000000015</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0.6440505192749999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.41648600246450002</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>0.20199571119528251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="E6:M6" si="1">CONCATENATE("(",F1,",",F5,"),")</f>
+        <v>(2025,1),</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2026,0.97),</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2027,0.9409),</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2028,0.912673),</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2029,0.88529281),</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2030,0.644050519275),</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2031,0.4164860024645),</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>(2032,0.201995711195283),</v>
+      </c>
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C7" t="str">
+        <f>CONCATENATE(C6,F6,G6,H6,I6,J6,K6,L6,M6,N6)</f>
+        <v>("Schedule 3",(2021,0),(2024,0),(2025,1),(2026,0.97),(2027,0.9409),(2028,0.912673),(2029,0.88529281),(2030,0.644050519275),(2031,0.4164860024645),(2032,0.201995711195283),(2033,0),(2050,0)),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>